<commit_message>
Table updates for V2 draft
</commit_message>
<xml_diff>
--- a/final-outputs/Raw Data 2019 Changes From Previous Years.xlsx
+++ b/final-outputs/Raw Data 2019 Changes From Previous Years.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\final-outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{819F49E4-2D86-4BAD-A1D9-93524AE63A39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B06DE27-92DC-4135-89BC-DA48EC758E54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data 2019" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,15 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Changes!$A$1:$AS$215</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Raw Data 2019'!$A$1:$AS$215</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -492,7 +500,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1000,71 +1008,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1102,44 +1046,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1466,14 +1372,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS215"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E185" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -30934,13 +30840,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS215">
+  <autoFilter ref="A1:AS215" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AS215">
       <sortCondition ref="C1:C215"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="E3:AS215">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>"e3!=e2"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30950,15 +30856,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AS215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E215" sqref="E215"/>
+      <selection pane="bottomRight" activeCell="T185" sqref="T185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -69152,18 +69058,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS215">
+  <autoFilter ref="A1:AS215" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="3">
       <filters>
         <filter val="2019"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AS215">
+      <sortCondition ref="C1:C215"/>
+    </sortState>
   </autoFilter>
   <conditionalFormatting sqref="E3:AS215">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>"e3!=e2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
@@ -69171,10 +69080,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>